<commit_message>
Commission Panels 1B and 1C
</commit_message>
<xml_diff>
--- a/UI/Channel_MQTT_Web_mapping.xlsx
+++ b/UI/Channel_MQTT_Web_mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="143">
   <si>
     <t xml:space="preserve">Panel</t>
   </si>
@@ -169,67 +169,88 @@
     <t xml:space="preserve">lighting/panel_1b/switch/channel_1</t>
   </si>
   <si>
-    <t xml:space="preserve">WestHallWesternOdds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Hall Western Odd Rows</t>
+    <t xml:space="preserve">WestHallAisles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Hall Aisle Rows</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_2</t>
   </si>
   <si>
-    <t xml:space="preserve">WestHallWesternEvens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Hall Western Even Rows</t>
+    <t xml:space="preserve">WestHallWestBayOdds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Hall West Bay Odd Rows</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_3</t>
   </si>
   <si>
+    <t xml:space="preserve">WestHallWestBayEvens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Hall West Bay Even Rows</t>
+  </si>
+  <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_4</t>
   </si>
   <si>
+    <t xml:space="preserve">WestHallMidBaySouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Hall Mid Bay South Rows</t>
+  </si>
+  <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_5</t>
   </si>
   <si>
-    <t xml:space="preserve">WestHallMiddleOdds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Hall Middle Odd Rows</t>
+    <t xml:space="preserve">WestHallMidBayNorth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Hall Mid Bay North Rows</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_6</t>
   </si>
   <si>
-    <t xml:space="preserve">WestHallMiddleEvens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Hall Middle Even Rows</t>
+    <t xml:space="preserve">WestHallEastBayNorth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Hall East Bay North Rows</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_7</t>
   </si>
   <si>
+    <t xml:space="preserve">WestHallEastBaySouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Hall East Bay South Rows</t>
+  </si>
+  <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_8</t>
   </si>
   <si>
+    <t xml:space="preserve">West Hall West Window South Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/ds4/lux</t>
+  </si>
+  <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_9</t>
   </si>
   <si>
-    <t xml:space="preserve">WestHallEasternOdds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Hall Eastern Odd Rows</t>
+    <t xml:space="preserve">West Hall West Window North Row</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_10</t>
   </si>
   <si>
-    <t xml:space="preserve">WestHallEasternEvens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Hall Eastern Even Rows</t>
+    <t xml:space="preserve">West Hall North Window Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/ds5/lux</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_11</t>
@@ -241,18 +262,9 @@
     <t xml:space="preserve">lighting/panel_1b/switch/channel_13</t>
   </si>
   <si>
-    <t xml:space="preserve">West Hall Northern Window Row</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/ds4/lux</t>
-  </si>
-  <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_14</t>
   </si>
   <si>
-    <t xml:space="preserve">West Hall Western Window Row</t>
-  </si>
-  <si>
     <t xml:space="preserve">lighting/panel_1b/switch/channel_15</t>
   </si>
   <si>
@@ -265,13 +277,94 @@
     <t xml:space="preserve">lighting/panel_1c/switch/channel_1</t>
   </si>
   <si>
+    <t xml:space="preserve">EastHallWestBayNorthOdds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Hall West Bay North Odd Rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallWestBaySouthOdds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Hall West Bay South Odd Rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallWestBayNorthEvens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Hall West Bay North Even Rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallWestBaySouthEvens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Hall West Bay South Even Rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallEastBayNorthOdds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallEastBaySouthOdds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallEastBayNorthEvens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallEastBaySouthEvens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallSouthEastBayEvens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EastHallSouthEastBayOdds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercantile Window Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/ds6/lux</t>
+  </si>
+  <si>
     <t xml:space="preserve">MercantileOdds</t>
   </si>
   <si>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mercantile Odd Rows</t>
   </si>
   <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_2</t>
+    <t xml:space="preserve">lighting/panel_1c/switch/channel_13</t>
   </si>
   <si>
     <t xml:space="preserve">MercantileEvens</t>
@@ -280,82 +373,7 @@
     <t xml:space="preserve">Mercantile Even Rows</t>
   </si>
   <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercantile Window Row</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/ds6/lux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EastHallWesternOdds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Hall Western Odd Rows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EastHallWesternEvens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Hall Western Even Rows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EastHallEasternOdds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Hall Eastern Odd Rows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EastHallEasternEvens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Hall Eastern Even Rows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/panel_1c/switch/channel_13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HotMetalOdds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hot Metal Areas Odd Rows</t>
-  </si>
-  <si>
     <t xml:space="preserve">lighting/panel_1c/switch/channel_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HotMetalEvens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hot Metal Areas Even Rows</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1c/switch/channel_15</t>
@@ -440,13 +458,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -465,14 +482,90 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,20 +574,62 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFF8CBAD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFBDD7EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFBDD7EE"/>
-        <bgColor rgb="FFC5E0B4"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
-        <bgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
-        <bgColor rgb="FFFFE699"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -504,7 +639,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -512,8 +647,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -537,6 +687,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -547,69 +748,86 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC5E0B4"/>
@@ -617,7 +835,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -635,7 +853,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFE699"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF8CBAD"/>
       <rgbColor rgb="FF3366FF"/>
@@ -666,8 +884,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15:E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="43:43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1015,7 +1233,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>47</v>
       </c>
@@ -1035,7 +1253,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
@@ -1055,7 +1273,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>47</v>
       </c>
@@ -1065,13 +1283,17 @@
       <c r="C20" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
@@ -1079,15 +1301,19 @@
         <v>4</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
         <v>47</v>
       </c>
@@ -1095,19 +1321,19 @@
         <v>5</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
         <v>47</v>
       </c>
@@ -1115,19 +1341,19 @@
         <v>6</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
         <v>47</v>
       </c>
@@ -1135,15 +1361,19 @@
         <v>7</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
         <v>47</v>
       </c>
@@ -1151,15 +1381,23 @@
         <v>8</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>47</v>
       </c>
@@ -1167,19 +1405,23 @@
         <v>9</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>65</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
         <v>47</v>
       </c>
@@ -1187,19 +1429,23 @@
         <v>10</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>68</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>75</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
         <v>47</v>
       </c>
@@ -1207,7 +1453,7 @@
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1215,7 +1461,7 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
         <v>47</v>
       </c>
@@ -1223,7 +1469,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1231,7 +1477,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
         <v>47</v>
       </c>
@@ -1239,23 +1485,15 @@
         <v>13</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
         <v>47</v>
       </c>
@@ -1263,21 +1501,13 @@
         <v>14</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
@@ -1287,7 +1517,7 @@
         <v>15</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1303,7 +1533,7 @@
         <v>16</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1311,41 +1541,41 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B34" s="8" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B35" s="8" t="n">
         <v>2</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
@@ -1353,235 +1583,247 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B36" s="8" t="n">
         <v>3</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="8"/>
+        <v>90</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="E36" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>81</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B37" s="8" t="n">
         <v>4</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+        <v>93</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B38" s="8" t="n">
         <v>5</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B39" s="8" t="n">
         <v>6</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B40" s="8" t="n">
         <v>7</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+        <v>100</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B41" s="8" t="n">
         <v>8</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B42" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>100</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B43" s="8" t="n">
         <v>10</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>103</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B44" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
+      <c r="E44" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B45" s="8" t="n">
         <v>12</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B46" s="8" t="n">
         <v>13</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B47" s="8" t="n">
         <v>14</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>111</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B48" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
@@ -1589,15 +1831,15 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B49" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -1607,19 +1849,19 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B50" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
@@ -1627,19 +1869,19 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B51" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
@@ -1647,35 +1889,35 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B52" s="10" t="n">
         <v>3</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G52" s="10" t="s">
         <v>122</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="H52" s="10"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B53" s="10" t="n">
         <v>4</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
@@ -1685,13 +1927,13 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B54" s="10" t="n">
         <v>5</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
@@ -1701,13 +1943,13 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B55" s="10" t="n">
         <v>6</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
@@ -1717,13 +1959,13 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B56" s="10" t="n">
         <v>7</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
@@ -1733,13 +1975,13 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B57" s="10" t="n">
         <v>8</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
@@ -1749,13 +1991,13 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B58" s="10" t="n">
         <v>9</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
@@ -1765,13 +2007,13 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B59" s="10" t="n">
         <v>10</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
@@ -1781,13 +2023,13 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B60" s="10" t="n">
         <v>11</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
@@ -1797,13 +2039,13 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B61" s="10" t="n">
         <v>12</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
@@ -1813,13 +2055,13 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B62" s="10" t="n">
         <v>13</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
@@ -1829,13 +2071,13 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B63" s="10" t="n">
         <v>14</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
@@ -1845,13 +2087,13 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B64" s="10" t="n">
         <v>15</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
@@ -1861,13 +2103,13 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B65" s="10" t="n">
         <v>16</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>

</xml_diff>